<commit_message>
Added new OrderDetails class inside utility
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9335"/>
+    <workbookView windowWidth="22368" windowHeight="9335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="product_details" sheetId="2" r:id="rId2"/>
+    <sheet name="shipping_address" sheetId="3" r:id="rId3"/>
+    <sheet name="credit_card" sheetId="4" r:id="rId4"/>
+    <sheet name="account_details" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>username</t>
   </si>
@@ -56,6 +60,141 @@
   </si>
   <si>
     <t>Tpcweb126</t>
+  </si>
+  <si>
+    <t>systemName</t>
+  </si>
+  <si>
+    <t>systemCategory</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>kitName</t>
+  </si>
+  <si>
+    <t>ProactivMD</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30-day</t>
+  </si>
+  <si>
+    <t>Acne Scar Duo</t>
+  </si>
+  <si>
+    <t>Proactiv Solution</t>
+  </si>
+  <si>
+    <t>90-day</t>
+  </si>
+  <si>
+    <t>Oil Control Duo</t>
+  </si>
+  <si>
+    <t>Proactiv+</t>
+  </si>
+  <si>
+    <t>3-piece system</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>Tpc</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>620 8th Ave</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Next Day</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>cardtype</t>
+  </si>
+  <si>
+    <t>cardno</t>
+  </si>
+  <si>
+    <t>cardname</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>cvv</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>5405222222222226</t>
+  </si>
+  <si>
+    <t>TPC Card</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>AMEX</t>
+  </si>
+  <si>
+    <t>343434343434343</t>
+  </si>
+  <si>
+    <t>DISCOVER</t>
+  </si>
+  <si>
+    <t>6011111111111117</t>
+  </si>
+  <si>
+    <t>emailID</t>
+  </si>
+  <si>
+    <t>tpc_test_12740@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -63,9 +202,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -77,6 +216,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,17 +233,54 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -108,53 +292,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,6 +309,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -184,14 +339,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -199,31 +361,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,19 +383,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,37 +497,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,133 +567,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -455,9 +607,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,27 +632,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,16 +671,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,160 +705,167 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,8 +1187,8 @@
   <sheetPr/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1039,46 +1198,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1086,54 +1245,54 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1141,4 +1300,358 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="20.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="3" max="4" width="13.8888888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="7"/>
+  <cols>
+    <col min="3" max="3" width="11.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="9.55555555555556" customWidth="1"/>
+    <col min="7" max="7" width="11.7777777777778"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="6">
+        <v>10018</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3103103100</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="8:8">
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="8:8">
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2022</v>
+      </c>
+      <c r="F2" s="6">
+        <v>111</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="3:8">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="27.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="11.1111111111111" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="3:8">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="tpc_test_12740@yopmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new data in Data.xlsx
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -202,9 +202,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -246,55 +246,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,8 +285,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -318,6 +302,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,20 +324,27 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -354,15 +353,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,13 +389,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,31 +491,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,127 +545,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,17 +605,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -627,6 +616,54 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,204 +686,167 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -855,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1602,7 +1602,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>

</xml_diff>